<commit_message>
update db for mysql
</commit_message>
<xml_diff>
--- a/doc/rest.xlsx
+++ b/doc/rest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
   <si>
     <t>Entity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -91,18 +91,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>JSON</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Operator</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>JSON</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Promotion</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -176,6 +168,30 @@
   </si>
   <si>
     <t>get promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object of tenant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object of tenant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Objects of tenant</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object of Operator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object of Promotion</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSON Object of PromotionBalance</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -566,7 +582,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -616,6 +632,9 @@
         <f>Server&amp;"/admin/tenant"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
       </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
       <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
@@ -634,6 +653,9 @@
         <f>Server&amp;"/admin/tenant"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
       </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
@@ -650,7 +672,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant/{tenantId}</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -668,12 +690,12 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -685,10 +707,13 @@
         <f>Server&amp;"/admin/operator"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -700,10 +725,13 @@
         <f>Server&amp;"/admin/operator"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -716,12 +744,12 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
@@ -734,12 +762,12 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
@@ -751,10 +779,13 @@
         <f>Server&amp;"/admin/promotion"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
       </c>
+      <c r="E10" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -766,10 +797,13 @@
         <f>Server&amp;"/admin/promotion"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
       </c>
+      <c r="E11" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -782,12 +816,12 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}/{promotionId}</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -800,12 +834,12 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -817,13 +851,16 @@
         <f>Server&amp;"/admin/promotionbalance/{promotionId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotionbalance/{promotionId}</v>
       </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -838,10 +875,10 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C22" t="s">
         <v>14</v>
@@ -853,10 +890,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C23" t="s">
         <v>14</v>
@@ -868,10 +905,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -883,10 +920,10 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -898,28 +935,28 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D26" t="str">
         <f>Server&amp;"/public/getbonus/{tenantId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/getbonus/{tenantId}</v>
       </c>
       <c r="E26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
         <v>13</v>
@@ -929,15 +966,15 @@
         <v>http://127.0.0.1:8080/vol-appserver/public/sendbonus/{tenantId}</v>
       </c>
       <c r="E27" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -947,15 +984,15 @@
         <v>http://127.0.0.1:8080/vol-appserver/public/activebonus/{tenantId}</v>
       </c>
       <c r="E28" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
         <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>28</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -967,10 +1004,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -982,10 +1019,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
@@ -997,10 +1034,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
support query bonus and quota by username
</commit_message>
<xml_diff>
--- a/doc/rest.xlsx
+++ b/doc/rest.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Entity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -151,10 +151,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>bonusId=$bonusId&amp;userId=$userId</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>bonusId=$bonusId</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -192,6 +188,18 @@
   </si>
   <si>
     <t>JSON Object of PromotionBalance</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>list quota by username</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>list bonus by username</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>bonusId=$bonusId&amp;toUser={toUserName}&amp;fromUser={fromUserName}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -578,17 +586,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="30.125" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="2" max="2" width="25.25" customWidth="1"/>
     <col min="3" max="3" width="14.125" customWidth="1"/>
     <col min="4" max="4" width="99.875" customWidth="1"/>
     <col min="5" max="5" width="30.375" customWidth="1"/>
@@ -633,7 +641,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
       </c>
       <c r="E2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>17</v>
@@ -650,11 +658,11 @@
         <v>13</v>
       </c>
       <c r="D3" t="str">
-        <f>Server&amp;"/admin/tenant"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
+        <f>Server&amp;"/admin/tenant/{tenantId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/tenant/{tenantId}</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.15">
@@ -672,7 +680,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant/{tenantId}</v>
       </c>
       <c r="F4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.15">
@@ -690,7 +698,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/tenant</v>
       </c>
       <c r="F5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
@@ -708,7 +716,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -722,11 +730,11 @@
         <v>13</v>
       </c>
       <c r="D7" t="str">
-        <f>Server&amp;"/admin/operator"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
+        <f>Server&amp;"/admin/operator/{operatorId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.15">
@@ -744,7 +752,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
       </c>
       <c r="F8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.15">
@@ -762,7 +770,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.15">
@@ -780,7 +788,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
@@ -798,7 +806,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
       </c>
       <c r="E11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -816,7 +824,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}/{promotionId}</v>
       </c>
       <c r="F12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.15">
@@ -830,11 +838,11 @@
         <v>15</v>
       </c>
       <c r="D13" t="str">
-        <f>Server&amp;"/admin/promotion/{tenantId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}</v>
+        <f>Server&amp;"/admin/promotion/{tenantId}/{promotionId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}/{promotionId}</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.15">
@@ -852,7 +860,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotionbalance/{promotionId}</v>
       </c>
       <c r="F14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -908,7 +916,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>14</v>
@@ -923,7 +931,7 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -948,7 +956,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/public/getbonus/{tenantId}</v>
       </c>
       <c r="E26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.15">
@@ -966,7 +974,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/public/sendbonus/{tenantId}</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.15">
@@ -984,7 +992,7 @@
         <v>http://127.0.0.1:8080/vol-appserver/public/activebonus/{tenantId}</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.15">
@@ -1004,17 +1012,17 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
       </c>
       <c r="D30" t="str">
-        <f>Server&amp;"/public/bonus/{tenantId}/{userId}/{bonusId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}/{userId}/{bonusId}</v>
+        <f>Server&amp;"/public/bonus/{tenantId}?userName={userName}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}?userName={userName}</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.15">
@@ -1022,14 +1030,14 @@
         <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" t="s">
         <v>14</v>
       </c>
       <c r="D31" t="str">
-        <f>Server&amp;"/public/quota/{tenantId}/{userId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}</v>
+        <f>Server&amp;"/public/bonus/{tenantId}/{userId}/{bonusId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}/{userId}/{bonusId}</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.15">
@@ -1037,12 +1045,42 @@
         <v>24</v>
       </c>
       <c r="B32" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="str">
+        <f>Server&amp;"/public/quota/{tenantId}/{userId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33" t="str">
+        <f>Server&amp;"/public/quota/{tenantId}?userName={userName}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}?userName={userName}</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" t="str">
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="str">
         <f>Server&amp;"/public/quota/{tenantId}/{userId}/{quotaId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}/{quotaId}</v>
       </c>

</xml_diff>

<commit_message>
support query by name
</commit_message>
<xml_diff>
--- a/doc/rest.xlsx
+++ b/doc/rest.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>Entity</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -200,6 +200,18 @@
   </si>
   <si>
     <t>bonusId=$bonusId&amp;toUser={toUserName}&amp;fromUser={fromUserName}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List by name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>List by name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>get User Info by name</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -586,11 +598,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N34"/>
+  <dimension ref="A1:N37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -703,20 +715,20 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D6" t="str">
-        <f>Server&amp;"/admin/operator"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
-      </c>
-      <c r="E6" t="s">
-        <v>40</v>
+        <f>Server&amp;"/admin/tenant?query=byName&amp;name={Name}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/tenant?query=byName&amp;name={Name}</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.15">
@@ -724,14 +736,14 @@
         <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" t="str">
-        <f>Server&amp;"/admin/operator/{operatorId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
+        <f>Server&amp;"/admin/operator"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -742,16 +754,16 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="str">
         <f>Server&amp;"/admin/operator/{operatorId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
       </c>
-      <c r="F8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -760,53 +772,53 @@
         <v>18</v>
       </c>
       <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="str">
+        <f>Server&amp;"/admin/operator/{operatorId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/operator/{operatorId}</v>
+      </c>
+      <c r="F9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="str">
+      <c r="D10" t="str">
         <f>Server&amp;"/admin/operator"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/operator</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="str">
-        <f>Server&amp;"/admin/promotion"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
-      </c>
-      <c r="E10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D11" t="str">
-        <f>Server&amp;"/admin/promotion"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
-      </c>
-      <c r="E11" t="s">
-        <v>41</v>
+        <f>Server&amp;"/admin/operator?query=byName&amp;name={Name}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/operator?query=byName&amp;name={Name}</v>
+      </c>
+      <c r="F11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.15">
@@ -814,16 +826,16 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D12" t="str">
-        <f>Server&amp;"/admin/promotion/{tenantId}/{promotionId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}/{promotionId}</v>
-      </c>
-      <c r="F12" t="s">
+        <f>Server&amp;"/admin/promotion"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
+      </c>
+      <c r="E12" t="s">
         <v>41</v>
       </c>
     </row>
@@ -832,35 +844,35 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D13" t="str">
+        <f>Server&amp;"/admin/promotion"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion</v>
+      </c>
+      <c r="E13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14" t="str">
         <f>Server&amp;"/admin/promotion/{tenantId}/{promotionId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}/{promotionId}</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F14" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.15">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" t="str">
-        <f>Server&amp;"/admin/promotionbalance/{promotionId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/admin/promotionbalance/{promotionId}</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.15">
@@ -868,191 +880,200 @@
         <v>19</v>
       </c>
       <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="str">
+        <f>Server&amp;"/admin/promotion/{tenantId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16" t="str">
+        <f>Server&amp;"/admin/promotion/{tenantId}?query=byName&amp;name={Name}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/{tenantId}?query=byName&amp;name={Name}</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="str">
+        <f>Server&amp;"/admin/promotionbalance/{promotionId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/admin/promotionbalance/{promotionId}</v>
+      </c>
+      <c r="F17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
         <v>32</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>13</v>
       </c>
-      <c r="D15" t="str">
+      <c r="D18" t="str">
         <f>Server&amp;"/admin/promotion/active/{promotionId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/admin/promotion/active/{promotionId}</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A18" s="3"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A21" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B25" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="str">
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" t="str">
         <f>Server&amp;"/public/user/{tenantId}/{userId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/user/{tenantId}/{userId}</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A26" t="s">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
-        <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="str">
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" t="str">
         <f>Server&amp;"/public/user/{tenantId}?query=byName&amp;name={userName}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/user/{tenantId}?query=byName&amp;name={userName}</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A27" t="s">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B27" t="s">
         <v>35</v>
       </c>
-      <c r="C24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="str">
+      <c r="C27" t="s">
+        <v>14</v>
+      </c>
+      <c r="D27" t="str">
         <f>Server&amp;"/public/promotion/{tenantId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/promotion/{tenantId}</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A25" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>36</v>
       </c>
-      <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="str">
+      <c r="C28" t="s">
+        <v>14</v>
+      </c>
+      <c r="D28" t="str">
         <f>Server&amp;"/public/promotion/{tenantId}/{promotionId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/promotion/{tenantId}/{promotionId}</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A26" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A29" t="s">
         <v>22</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B29" t="s">
         <v>27</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C29" t="s">
         <v>20</v>
       </c>
-      <c r="D26" t="str">
+      <c r="D29" t="str">
         <f>Server&amp;"/public/getbonus/{tenantId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/getbonus/{tenantId}</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E29" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C30" t="s">
         <v>13</v>
       </c>
-      <c r="D27" t="str">
+      <c r="D30" t="str">
         <f>Server&amp;"/public/sendbonus/{tenantId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/sendbonus/{tenantId}</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A31" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B31" t="s">
         <v>25</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C31" t="s">
         <v>13</v>
       </c>
-      <c r="D28" t="str">
+      <c r="D31" t="str">
         <f>Server&amp;"/public/activebonus/{tenantId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/activebonus/{tenantId}</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E31" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="A32" t="s">
         <v>24</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B32" t="s">
         <v>26</v>
       </c>
-      <c r="C29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" t="str">
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32" t="str">
         <f>Server&amp;"/public/bonus/{tenantId}/{userId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}/{userId}</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" t="s">
-        <v>44</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" t="str">
-        <f>Server&amp;"/public/bonus/{tenantId}?userName={userName}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}?userName={userName}</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" t="s">
-        <v>28</v>
-      </c>
-      <c r="C31" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" t="str">
-        <f>Server&amp;"/public/bonus/{tenantId}/{userId}/{bonusId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}/{userId}/{bonusId}</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" t="s">
-        <v>24</v>
-      </c>
-      <c r="B32" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" t="str">
-        <f>Server&amp;"/public/quota/{tenantId}/{userId}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -1060,14 +1081,14 @@
         <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C33" t="s">
         <v>14</v>
       </c>
       <c r="D33" t="str">
-        <f>Server&amp;"/public/quota/{tenantId}?userName={userName}"</f>
-        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}?userName={userName}</v>
+        <f>Server&amp;"/public/bonus/{tenantId}?userName={userName}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}?userName={userName}</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.15">
@@ -1075,12 +1096,57 @@
         <v>24</v>
       </c>
       <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" t="str">
+        <f>Server&amp;"/public/bonus/{tenantId}/{userId}/{bonusId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/bonus/{tenantId}/{userId}/{bonusId}</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35" t="str">
+        <f>Server&amp;"/public/quota/{tenantId}/{userId}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A36" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="str">
+        <f>Server&amp;"/public/quota/{tenantId}?userName={userName}"</f>
+        <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}?userName={userName}</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
         <v>30</v>
       </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" t="str">
+      <c r="C37" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" t="str">
         <f>Server&amp;"/public/quota/{tenantId}/{userId}/{quotaId}"</f>
         <v>http://127.0.0.1:8080/vol-appserver/public/quota/{tenantId}/{userId}/{quotaId}</v>
       </c>
@@ -1089,7 +1155,7 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="N2" r:id="rId1"/>
-    <hyperlink ref="E28" r:id="rId2" display="bonusId=$bonusId@userName=$userName"/>
+    <hyperlink ref="E31" r:id="rId2" display="bonusId=$bonusId@userName=$userName"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>